<commit_message>
add new package to requirement
</commit_message>
<xml_diff>
--- a/course/excel/transactions_modified.xlsx
+++ b/course/excel/transactions_modified.xlsx
@@ -377,7 +377,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.55€</t>
+          <t>5,36 €</t>
         </is>
       </c>
     </row>
@@ -395,7 +395,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7.65€</t>
+          <t>6,25 €</t>
         </is>
       </c>
     </row>
@@ -413,7 +413,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8.75€</t>
+          <t>7,16 €</t>
         </is>
       </c>
     </row>

</xml_diff>